<commit_message>
Improve parsing of tournament schedules and add match search functionality
Update `pdf-to-excel.ts` to improve category detection and match parsing logic. Introduce `server/search-match.ts` to read and search for specific matches within an Excel file using the `xlsx` library.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 2336cc0f-0422-4bc3-a4a5-c7aa546b01f5
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/b058bf07-84cc-41ad-b409-5c39e27e4fce/2336cc0f-0422-4bc3-a4a5-c7aa546b01f5/vG40gau
</commit_message>
<xml_diff>
--- a/public/cronograma_25_oct.xlsx
+++ b/public/cronograma_25_oct.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -453,22 +453,22 @@
         <v>Múltiples canchas</v>
       </c>
       <c r="D2" t="str">
-        <v>SUMA 9 FEMENIL</v>
+        <v>SUMA 5 VARONIL</v>
       </c>
       <c r="E2" t="str">
-        <v>Jornada 1</v>
+        <v>Jornada 3</v>
       </c>
       <c r="F2" t="str">
-        <v>Queta Izaguirre</v>
+        <v>Daniel De Jesus Ortiz</v>
       </c>
       <c r="G2" t="str">
-        <v>Ivonne María Pérez</v>
+        <v>Agustin I. Gil</v>
       </c>
       <c r="H2" t="str">
-        <v>Claudia Valenciana</v>
+        <v>Carlos Manjarrez</v>
       </c>
       <c r="I2" t="str">
-        <v>Ana Marcela Ortega</v>
+        <v>Emiliano Sánchez</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +476,7 @@
         <v>2025-10-26</v>
       </c>
       <c r="B3" t="str">
-        <v>09:30</v>
+        <v>08:15</v>
       </c>
       <c r="C3" t="str">
         <v>Múltiples canchas</v>
@@ -485,19 +485,19 @@
         <v>SUMA 9 FEMENIL</v>
       </c>
       <c r="E3" t="str">
-        <v>Jornada 2</v>
+        <v>Jornada 1</v>
       </c>
       <c r="F3" t="str">
-        <v>Sonia Anaya</v>
+        <v>Queta Izaguirre</v>
       </c>
       <c r="G3" t="str">
-        <v>Cecy Cardiel</v>
+        <v>Ivonne María Pérez</v>
       </c>
       <c r="H3" t="str">
-        <v>Martha Bustos</v>
+        <v>Claudia Valenciana</v>
       </c>
       <c r="I3" t="str">
-        <v>Sonia Garcia</v>
+        <v>Ana Marcela Ortega</v>
       </c>
     </row>
     <row r="4">
@@ -511,22 +511,22 @@
         <v>Múltiples canchas</v>
       </c>
       <c r="D4" t="str">
-        <v>SUMA 9 FEMENIL</v>
+        <v>SUMA 3 FEMENIL</v>
       </c>
       <c r="E4" t="str">
-        <v>Jornada 2</v>
+        <v>Jornada 1</v>
       </c>
       <c r="F4" t="str">
-        <v>Aranza Russek</v>
+        <v>Ana Lucia Cepeda</v>
       </c>
       <c r="G4" t="str">
-        <v>Maika Ramos</v>
+        <v>Regina Jaidar</v>
       </c>
       <c r="H4" t="str">
-        <v>Alejandra Martinez</v>
+        <v>Olivia Zúñiga</v>
       </c>
       <c r="I4" t="str">
-        <v>Ana Sofia Cabral</v>
+        <v>Susy Rivera</v>
       </c>
     </row>
     <row r="5">
@@ -540,22 +540,22 @@
         <v>Múltiples canchas</v>
       </c>
       <c r="D5" t="str">
-        <v>CUARTA VARONIL</v>
+        <v>SUMA 9 FEMENIL</v>
       </c>
       <c r="E5" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F5" t="str">
-        <v>Christian Orrin</v>
+        <v>Sonia Anaya</v>
       </c>
       <c r="G5" t="str">
-        <v>Antonio Albores</v>
+        <v>Cecy Cardiel</v>
       </c>
       <c r="H5" t="str">
-        <v>Adrián Gómez</v>
+        <v>Martha Bustos</v>
       </c>
       <c r="I5" t="str">
-        <v>Roberto Quezada</v>
+        <v>Sonia Garcia</v>
       </c>
     </row>
     <row r="6">
@@ -569,22 +569,22 @@
         <v>Múltiples canchas</v>
       </c>
       <c r="D6" t="str">
-        <v>SUMA 7 VARONIL</v>
+        <v>SUMA 9 FEMENIL</v>
       </c>
       <c r="E6" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F6" t="str">
-        <v>Pancho Ruiz</v>
+        <v>Aranza Russek</v>
       </c>
       <c r="G6" t="str">
-        <v>Eduardo Martinez</v>
+        <v>Maika Ramos</v>
       </c>
       <c r="H6" t="str">
-        <v>Ruben Diaz flores</v>
+        <v>Alejandra Martinez</v>
       </c>
       <c r="I6" t="str">
-        <v>Pablo Garza T.</v>
+        <v>Ana Sofia Cabral</v>
       </c>
     </row>
     <row r="7">
@@ -592,28 +592,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B7" t="str">
-        <v>10:45</v>
+        <v>09:30</v>
       </c>
       <c r="C7" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D7" t="str">
-        <v>SUMA 9 FEMENIL</v>
+        <v>CUARTA VARONIL</v>
       </c>
       <c r="E7" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F7" t="str">
-        <v>Cecilia Salmón</v>
+        <v>Christian Orrin</v>
       </c>
       <c r="G7" t="str">
-        <v>Emma Villarreal</v>
+        <v>Antonio Albores</v>
       </c>
       <c r="H7" t="str">
-        <v>Milagros Angeli Martinez</v>
+        <v>Adrián Gómez</v>
       </c>
       <c r="I7" t="str">
-        <v>Maria Valentina Galarza Hernández</v>
+        <v>Roberto Quezada</v>
       </c>
     </row>
     <row r="8">
@@ -621,28 +621,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B8" t="str">
-        <v>10:45</v>
+        <v>09:30</v>
       </c>
       <c r="C8" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D8" t="str">
-        <v>SUMA 9 FEMENIL</v>
+        <v>SUMA 7 VARONIL</v>
       </c>
       <c r="E8" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F8" t="str">
-        <v>Irma Murguía</v>
+        <v>Pancho Ruiz</v>
       </c>
       <c r="G8" t="str">
-        <v>Norma Zacarias</v>
+        <v>Eduardo Martinez</v>
       </c>
       <c r="H8" t="str">
-        <v>Luisanna Villarreal</v>
+        <v>Ruben Diaz flores</v>
       </c>
       <c r="I8" t="str">
-        <v>Melina Eguiarte</v>
+        <v>Pablo Garza T.</v>
       </c>
     </row>
     <row r="9">
@@ -656,22 +656,22 @@
         <v>Múltiples canchas</v>
       </c>
       <c r="D9" t="str">
-        <v>SUMA 7 VARONIL</v>
+        <v>SUMA 9 FEMENIL</v>
       </c>
       <c r="E9" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F9" t="str">
-        <v>Ricardo Garza</v>
+        <v>Sharon Angulo</v>
       </c>
       <c r="G9" t="str">
-        <v>Memo Rocha</v>
+        <v>Maria Fernanda Perez</v>
       </c>
       <c r="H9" t="str">
-        <v>Yan Fuentes</v>
+        <v>Melissa Eugenia Baca</v>
       </c>
       <c r="I9" t="str">
-        <v>Yoel Fuentes</v>
+        <v>Betty Baca</v>
       </c>
     </row>
     <row r="10">
@@ -685,22 +685,22 @@
         <v>Múltiples canchas</v>
       </c>
       <c r="D10" t="str">
-        <v>SUMA 7 VARONIL</v>
+        <v>SUMA 9 FEMENIL</v>
       </c>
       <c r="E10" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F10" t="str">
-        <v>Javier "Chipo" Cepeda</v>
+        <v>Cecilia Salmón</v>
       </c>
       <c r="G10" t="str">
-        <v>Luis Dibildox</v>
+        <v>Emma Villarreal</v>
       </c>
       <c r="H10" t="str">
-        <v>adrián fernandez</v>
+        <v>Milagros Angeli Martinez</v>
       </c>
       <c r="I10" t="str">
-        <v>Camilo Chaúl</v>
+        <v>Maria Valentina Galarza Hernández</v>
       </c>
     </row>
     <row r="11">
@@ -708,28 +708,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B11" t="str">
-        <v>12:00</v>
+        <v>10:45</v>
       </c>
       <c r="C11" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D11" t="str">
-        <v>SUMA 3 VARONIL</v>
+        <v>SUMA 9 FEMENIL</v>
       </c>
       <c r="E11" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F11" t="str">
-        <v>Armando Del Moral</v>
+        <v>Irma Murguía</v>
       </c>
       <c r="G11" t="str">
-        <v>Carlos Manjarrez</v>
+        <v>Norma Zacarias</v>
       </c>
       <c r="H11" t="str">
-        <v>German Madero</v>
+        <v>Luisanna Villarreal</v>
       </c>
       <c r="I11" t="str">
-        <v>Ruben Zapico</v>
+        <v>Melina Eguiarte</v>
       </c>
     </row>
     <row r="12">
@@ -737,28 +737,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B12" t="str">
-        <v>12:00</v>
+        <v>10:45</v>
       </c>
       <c r="C12" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D12" t="str">
-        <v>SUMA 3 VARONIL</v>
+        <v>SUMA 7 VARONIL</v>
       </c>
       <c r="E12" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F12" t="str">
-        <v>Angel Ramos</v>
+        <v>Ricardo Garza</v>
       </c>
       <c r="G12" t="str">
-        <v>Luis Emanuel Regalado</v>
+        <v>Memo Rocha</v>
       </c>
       <c r="H12" t="str">
-        <v>Mario Murguia</v>
+        <v>Yan Fuentes</v>
       </c>
       <c r="I12" t="str">
-        <v>Emmanuel Saldaña</v>
+        <v>Yoel Fuentes</v>
       </c>
     </row>
     <row r="13">
@@ -766,28 +766,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B13" t="str">
-        <v>12:00</v>
+        <v>10:45</v>
       </c>
       <c r="C13" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D13" t="str">
-        <v>SUMA 3 FEMENIL</v>
+        <v>SUMA 7 VARONIL</v>
       </c>
       <c r="E13" t="str">
-        <v>Jornada 3</v>
+        <v>Jornada 2</v>
       </c>
       <c r="F13" t="str">
-        <v>Ximena Robles</v>
+        <v>Javier "Chipo" Cepeda</v>
       </c>
       <c r="G13" t="str">
-        <v>Romina Batarse</v>
+        <v>Luis Dibildox</v>
       </c>
       <c r="H13" t="str">
-        <v>Isabella Cruz</v>
+        <v>adrián fernandez</v>
       </c>
       <c r="I13" t="str">
-        <v>Ivanna I Gutierrez</v>
+        <v>Camilo Chaúl</v>
       </c>
     </row>
     <row r="14">
@@ -804,19 +804,19 @@
         <v>SUMA 7 VARONIL</v>
       </c>
       <c r="E14" t="str">
-        <v>Jornada 2</v>
+        <v>Jornada 1</v>
       </c>
       <c r="F14" t="str">
-        <v>Ismael Cepeda</v>
+        <v>Alfredo Rodriguez</v>
       </c>
       <c r="G14" t="str">
-        <v>Israel García</v>
+        <v>Rodolfo Rios</v>
       </c>
       <c r="H14" t="str">
-        <v>José carlos Casas</v>
+        <v>Ruben Diaz flores</v>
       </c>
       <c r="I14" t="str">
-        <v>Fernando Pámanes</v>
+        <v>Pablo Garza T.</v>
       </c>
     </row>
     <row r="15">
@@ -824,28 +824,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B15" t="str">
-        <v>13:15</v>
+        <v>12:00</v>
       </c>
       <c r="C15" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D15" t="str">
-        <v>SUMA 7 VARONIL</v>
+        <v>SUMA 3 VARONIL</v>
       </c>
       <c r="E15" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F15" t="str">
-        <v>Fernando Perez</v>
+        <v>Armando Del Moral</v>
       </c>
       <c r="G15" t="str">
-        <v>Raul Urteaga</v>
+        <v>Carlos Manjarrez</v>
       </c>
       <c r="H15" t="str">
-        <v>Sergio Luna</v>
+        <v>German Madero</v>
       </c>
       <c r="I15" t="str">
-        <v>Rafael Caldera</v>
+        <v>Ruben Zapico</v>
       </c>
     </row>
     <row r="16">
@@ -853,28 +853,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B16" t="str">
-        <v>13:15</v>
+        <v>12:00</v>
       </c>
       <c r="C16" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D16" t="str">
-        <v>CUARTA VARONIL</v>
+        <v>SUMA 3 VARONIL</v>
       </c>
       <c r="E16" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F16" t="str">
-        <v>Salvador Cordova</v>
+        <v>Angel Ramos</v>
       </c>
       <c r="G16" t="str">
-        <v>Diego Cordova</v>
+        <v>Luis Emanuel Regalado</v>
       </c>
       <c r="H16" t="str">
-        <v>Jorge Castro</v>
+        <v>Mario Murguia</v>
       </c>
       <c r="I16" t="str">
-        <v>Diego Rivas</v>
+        <v>Emmanuel Saldaña</v>
       </c>
     </row>
     <row r="17">
@@ -882,28 +882,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B17" t="str">
-        <v>13:15</v>
+        <v>12:00</v>
       </c>
       <c r="C17" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D17" t="str">
-        <v>SUMA 7 VARONIL</v>
+        <v>SUMA 3 FEMENIL</v>
       </c>
       <c r="E17" t="str">
-        <v>Jornada 2</v>
+        <v>Jornada 3</v>
       </c>
       <c r="F17" t="str">
-        <v>Roberto Quezada</v>
+        <v>Ximena Robles</v>
       </c>
       <c r="G17" t="str">
-        <v>Martin Eduardo García</v>
+        <v>Romina Batarse</v>
       </c>
       <c r="H17" t="str">
-        <v>Ricardo "Jr" Garza</v>
+        <v>Isabella Cruz</v>
       </c>
       <c r="I17" t="str">
-        <v>Andres Garza</v>
+        <v>Ivanna I Gutierrez</v>
       </c>
     </row>
     <row r="18">
@@ -911,28 +911,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B18" t="str">
-        <v>13:15</v>
+        <v>12:00</v>
       </c>
       <c r="C18" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D18" t="str">
-        <v>CUARTA VARONIL</v>
+        <v>SUMA 7 VARONIL</v>
       </c>
       <c r="E18" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F18" t="str">
-        <v>Carlos Ibarra</v>
+        <v>Ismael Cepeda</v>
       </c>
       <c r="G18" t="str">
-        <v>Salvador Cordova</v>
+        <v>Israel García</v>
       </c>
       <c r="H18" t="str">
-        <v>Eugenio Salazar</v>
+        <v>José carlos Casas</v>
       </c>
       <c r="I18" t="str">
-        <v>Carlos Monarrez</v>
+        <v>Fernando Pámanes</v>
       </c>
     </row>
     <row r="19">
@@ -940,28 +940,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B19" t="str">
-        <v>14:30</v>
+        <v>13:15</v>
       </c>
       <c r="C19" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D19" t="str">
-        <v>TERCERA VARONIL</v>
+        <v>SUMA 3 VARONIL</v>
       </c>
       <c r="E19" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F19" t="str">
-        <v>Jose Guillermo Soto</v>
+        <v>Alan Cepeda</v>
       </c>
       <c r="G19" t="str">
-        <v>Santiago Alatorre</v>
+        <v>Eduardo Benjamí Cepeda</v>
       </c>
       <c r="H19" t="str">
-        <v>Rai Gonzalez</v>
+        <v>Ricky Jr. Martínez</v>
       </c>
       <c r="I19" t="str">
-        <v>Alejandro Sierra</v>
+        <v>Jesus Martinez</v>
       </c>
     </row>
     <row r="20">
@@ -969,28 +969,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B20" t="str">
-        <v>14:30</v>
+        <v>13:15</v>
       </c>
       <c r="C20" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D20" t="str">
-        <v>TERCERA VARONIL</v>
+        <v>SUMA 7 VARONIL</v>
       </c>
       <c r="E20" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F20" t="str">
-        <v>Inaki Sahagun</v>
+        <v>Fernando Perez</v>
       </c>
       <c r="G20" t="str">
-        <v>Jorge Chaúl</v>
+        <v>Raul Urteaga</v>
       </c>
       <c r="H20" t="str">
-        <v>Erick Martos</v>
+        <v>Sergio Luna</v>
       </c>
       <c r="I20" t="str">
-        <v>Carlos Estrada</v>
+        <v>Rafael Caldera</v>
       </c>
     </row>
     <row r="21">
@@ -998,28 +998,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B21" t="str">
-        <v>14:30</v>
+        <v>13:15</v>
       </c>
       <c r="C21" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D21" t="str">
-        <v>TERCERA VARONIL</v>
+        <v>CUARTA VARONIL</v>
       </c>
       <c r="E21" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F21" t="str">
-        <v>Carlos Dueñez</v>
+        <v>Salvador Cordova</v>
       </c>
       <c r="G21" t="str">
-        <v>Jesus Cobos</v>
+        <v>Diego Cordova</v>
       </c>
       <c r="H21" t="str">
-        <v>Héctor Hernandez</v>
+        <v>Jorge Castro</v>
       </c>
       <c r="I21" t="str">
-        <v>Letmar Yair Infante</v>
+        <v>Diego Rivas</v>
       </c>
     </row>
     <row r="22">
@@ -1027,28 +1027,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B22" t="str">
-        <v>14:30</v>
+        <v>13:15</v>
       </c>
       <c r="C22" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D22" t="str">
-        <v>CUARTA VARONIL</v>
+        <v>SUMA 7 VARONIL</v>
       </c>
       <c r="E22" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F22" t="str">
-        <v>Jose Roberto Avalos</v>
+        <v>Roberto Quezada</v>
       </c>
       <c r="G22" t="str">
-        <v>Hugo Luis Cornu</v>
+        <v>Martin Eduardo García</v>
       </c>
       <c r="H22" t="str">
-        <v>Raúl Bautista</v>
+        <v>Ricardo "Jr" Garza</v>
       </c>
       <c r="I22" t="str">
-        <v>René Montiel</v>
+        <v>Andres Garza</v>
       </c>
     </row>
     <row r="23">
@@ -1056,28 +1056,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B23" t="str">
-        <v>15:45</v>
+        <v>13:15</v>
       </c>
       <c r="C23" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D23" t="str">
-        <v>TERCERA VARONIL</v>
+        <v>CUARTA VARONIL</v>
       </c>
       <c r="E23" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F23" t="str">
-        <v>Shafee Etemad Amini</v>
+        <v>Carlos Ibarra</v>
       </c>
       <c r="G23" t="str">
-        <v>Diego Monroy</v>
+        <v>Salvador Cordova</v>
       </c>
       <c r="H23" t="str">
-        <v>José carlos Casas</v>
+        <v>Eugenio Salazar</v>
       </c>
       <c r="I23" t="str">
-        <v>Ulberto Prieto</v>
+        <v>Carlos Monarrez</v>
       </c>
     </row>
     <row r="24">
@@ -1085,28 +1085,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B24" t="str">
-        <v>15:45</v>
+        <v>14:30</v>
       </c>
       <c r="C24" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D24" t="str">
-        <v>TERCERA FEMENIL</v>
+        <v>SUMA 3 VARONIL</v>
       </c>
       <c r="E24" t="str">
-        <v>Jornada 1</v>
+        <v>Jornada 2</v>
       </c>
       <c r="F24" t="str">
-        <v>Coquis Calderón</v>
+        <v>Diego Rosales</v>
       </c>
       <c r="G24" t="str">
-        <v>Marcela Aranda</v>
+        <v>Jose Peressini</v>
       </c>
       <c r="H24" t="str">
-        <v>Camila Becerra</v>
+        <v>Abraham “Abry”</v>
       </c>
       <c r="I24" t="str">
-        <v>Mariana Chávez</v>
+        <v>marco antonio rodriguez</v>
       </c>
     </row>
     <row r="25">
@@ -1114,7 +1114,7 @@
         <v>2025-10-26</v>
       </c>
       <c r="B25" t="str">
-        <v>15:45</v>
+        <v>14:30</v>
       </c>
       <c r="C25" t="str">
         <v>Múltiples canchas</v>
@@ -1126,16 +1126,16 @@
         <v>Jornada 2</v>
       </c>
       <c r="F25" t="str">
-        <v>Oscar Russek</v>
+        <v>Jose Guillermo Soto</v>
       </c>
       <c r="G25" t="str">
-        <v>Humberto Ruiz</v>
+        <v>Santiago Alatorre</v>
       </c>
       <c r="H25" t="str">
-        <v>Ismael Cepeda</v>
+        <v>Rai Gonzalez</v>
       </c>
       <c r="I25" t="str">
-        <v>Carlos "Mamirez Ramirez</v>
+        <v>Alejandro Sierra</v>
       </c>
     </row>
     <row r="26">
@@ -1143,7 +1143,7 @@
         <v>2025-10-26</v>
       </c>
       <c r="B26" t="str">
-        <v>15:45</v>
+        <v>14:30</v>
       </c>
       <c r="C26" t="str">
         <v>Múltiples canchas</v>
@@ -1155,16 +1155,16 @@
         <v>Jornada 2</v>
       </c>
       <c r="F26" t="str">
-        <v>Martin Eduardo García</v>
+        <v>Inaki Sahagun</v>
       </c>
       <c r="G26" t="str">
-        <v>Jesus Ramos</v>
+        <v>Jorge Chaúl</v>
       </c>
       <c r="H26" t="str">
-        <v>Patricio García</v>
+        <v>Erick Martos</v>
       </c>
       <c r="I26" t="str">
-        <v>Venancio Garcia</v>
+        <v>Carlos Estrada</v>
       </c>
     </row>
     <row r="27">
@@ -1172,28 +1172,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B27" t="str">
-        <v>17:00</v>
+        <v>14:30</v>
       </c>
       <c r="C27" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D27" t="str">
-        <v>SUMA 3 FEMENIL</v>
+        <v>TERCERA VARONIL</v>
       </c>
       <c r="E27" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F27" t="str">
-        <v>Karen Plata</v>
+        <v>Carlos Dueñez</v>
       </c>
       <c r="G27" t="str">
-        <v>Yamila Anahi de Maiquez</v>
+        <v>Jesus Cobos</v>
       </c>
       <c r="H27" t="str">
-        <v>Begoña Zarragoicoechea</v>
+        <v>Héctor Hernandez</v>
       </c>
       <c r="I27" t="str">
-        <v>Eugenia Martinez</v>
+        <v>Letmar Yair Infante</v>
       </c>
     </row>
     <row r="28">
@@ -1201,28 +1201,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B28" t="str">
-        <v>17:00</v>
+        <v>14:30</v>
       </c>
       <c r="C28" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D28" t="str">
-        <v>SUMA 3 FEMENIL</v>
+        <v>CUARTA VARONIL</v>
       </c>
       <c r="E28" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F28" t="str">
-        <v>Paola Tumoine</v>
+        <v>Jose Roberto Avalos</v>
       </c>
       <c r="G28" t="str">
-        <v>Liliana Tumoine</v>
+        <v>Hugo Luis Cornu</v>
       </c>
       <c r="H28" t="str">
-        <v>Olivia Zúñiga</v>
+        <v>Raúl Bautista</v>
       </c>
       <c r="I28" t="str">
-        <v>Susy Rivera</v>
+        <v>René Montiel</v>
       </c>
     </row>
     <row r="29">
@@ -1230,28 +1230,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B29" t="str">
-        <v>17:00</v>
+        <v>15:45</v>
       </c>
       <c r="C29" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D29" t="str">
-        <v>SUMA 5 VARONIL</v>
+        <v>QUINTA VARONIL</v>
       </c>
       <c r="E29" t="str">
-        <v>Jornada 2</v>
+        <v>Jornada 1</v>
       </c>
       <c r="F29" t="str">
-        <v>Josué Sánchez</v>
+        <v>Luis Robles</v>
       </c>
       <c r="G29" t="str">
-        <v>Patricio Murguia</v>
+        <v>Hector Molina</v>
       </c>
       <c r="H29" t="str">
-        <v>Hugo Facio</v>
+        <v>ALFREDO PADILLA</v>
       </c>
       <c r="I29" t="str">
-        <v>Eduardo Marin</v>
+        <v>Luis Daniel Salazar</v>
       </c>
     </row>
     <row r="30">
@@ -1259,28 +1259,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B30" t="str">
-        <v>17:00</v>
+        <v>15:45</v>
       </c>
       <c r="C30" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D30" t="str">
-        <v>SUMA 5 VARONIL</v>
+        <v>TERCERA VARONIL</v>
       </c>
       <c r="E30" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F30" t="str">
-        <v>Rafael Reyes</v>
+        <v>Shafee Etemad Amini</v>
       </c>
       <c r="G30" t="str">
-        <v>Andoni Esquivel</v>
+        <v>Diego Monroy</v>
       </c>
       <c r="H30" t="str">
-        <v>El Javi Fuentes</v>
+        <v>José carlos Casas</v>
       </c>
       <c r="I30" t="str">
-        <v>Hector Becerra</v>
+        <v>Ulberto Prieto</v>
       </c>
     </row>
     <row r="31">
@@ -1288,28 +1288,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B31" t="str">
-        <v>18:15</v>
+        <v>15:45</v>
       </c>
       <c r="C31" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D31" t="str">
-        <v>SUMA 1 VARONIL</v>
+        <v>TERCERA FEMENIL</v>
       </c>
       <c r="E31" t="str">
-        <v>Jornada 2</v>
+        <v>Jornada 1</v>
       </c>
       <c r="F31" t="str">
-        <v>Marco Estefania</v>
+        <v>Coquis Calderón</v>
       </c>
       <c r="G31" t="str">
-        <v>Andres Ollivier</v>
+        <v>Marcela Aranda</v>
       </c>
       <c r="H31" t="str">
-        <v>Juan Francisco González</v>
+        <v>Camila Becerra</v>
       </c>
       <c r="I31" t="str">
-        <v>Mauricio Batres</v>
+        <v>Mariana Chávez</v>
       </c>
     </row>
     <row r="32">
@@ -1317,28 +1317,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B32" t="str">
-        <v>18:15</v>
+        <v>15:45</v>
       </c>
       <c r="C32" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D32" t="str">
-        <v>SUMA 3 FEMENIL</v>
+        <v>TERCERA VARONIL</v>
       </c>
       <c r="E32" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F32" t="str">
-        <v>Daniela Peters</v>
+        <v>Oscar Russek</v>
       </c>
       <c r="G32" t="str">
-        <v>Sandra Martinez</v>
+        <v>Humberto Ruiz</v>
       </c>
       <c r="H32" t="str">
-        <v>amina cassani</v>
+        <v>Ismael Cepeda</v>
       </c>
       <c r="I32" t="str">
-        <v>Andrea Quintero</v>
+        <v>Carlos "Mamirez Ramirez</v>
       </c>
     </row>
     <row r="33">
@@ -1346,28 +1346,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B33" t="str">
-        <v>18:15</v>
+        <v>15:45</v>
       </c>
       <c r="C33" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D33" t="str">
-        <v>SUMA 5 VARONIL</v>
+        <v>TERCERA VARONIL</v>
       </c>
       <c r="E33" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F33" t="str">
-        <v>adrián fernandez</v>
+        <v>Martin Eduardo García</v>
       </c>
       <c r="G33" t="str">
-        <v>Roberto Soto</v>
+        <v>Jesus Ramos</v>
       </c>
       <c r="H33" t="str">
-        <v>Fernando Gilio</v>
+        <v>Patricio García</v>
       </c>
       <c r="I33" t="str">
-        <v>Diego Rosales</v>
+        <v>Venancio Garcia</v>
       </c>
     </row>
     <row r="34">
@@ -1375,28 +1375,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B34" t="str">
-        <v>18:15</v>
+        <v>17:00</v>
       </c>
       <c r="C34" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D34" t="str">
-        <v>SUMA 5 VARONIL</v>
+        <v>SUMA 3 FEMENIL</v>
       </c>
       <c r="E34" t="str">
-        <v>Jornada 2</v>
+        <v>Jornada 3</v>
       </c>
       <c r="F34" t="str">
-        <v>Carlos Mena</v>
+        <v>Ana Lucia</v>
       </c>
       <c r="G34" t="str">
-        <v>Elias Martinez</v>
+        <v>Cecy Garza</v>
       </c>
       <c r="H34" t="str">
-        <v>Mauricio Guizar</v>
+        <v>Regina Flores</v>
       </c>
       <c r="I34" t="str">
-        <v>Humberto Ruiz</v>
+        <v>Ana veronica Echavez</v>
       </c>
     </row>
     <row r="35">
@@ -1404,28 +1404,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B35" t="str">
-        <v>19:30</v>
+        <v>17:00</v>
       </c>
       <c r="C35" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D35" t="str">
-        <v>QUINTA VARONIL</v>
+        <v>SUMA 3 FEMENIL</v>
       </c>
       <c r="E35" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F35" t="str">
-        <v>Diego Fernandez</v>
+        <v>Karen Plata</v>
       </c>
       <c r="G35" t="str">
-        <v>Ale Ramos</v>
+        <v>Yamila Anahi de Maiquez</v>
       </c>
       <c r="H35" t="str">
-        <v>Raul Aguilar</v>
+        <v>Begoña Zarragoicoechea</v>
       </c>
       <c r="I35" t="str">
-        <v>Ernesto Sandoval</v>
+        <v>Eugenia Martinez</v>
       </c>
     </row>
     <row r="36">
@@ -1433,7 +1433,7 @@
         <v>2025-10-26</v>
       </c>
       <c r="B36" t="str">
-        <v>19:30</v>
+        <v>17:00</v>
       </c>
       <c r="C36" t="str">
         <v>Múltiples canchas</v>
@@ -1445,16 +1445,16 @@
         <v>Jornada 2</v>
       </c>
       <c r="F36" t="str">
-        <v>Isabella Cruz</v>
+        <v>Paola Tumoine</v>
       </c>
       <c r="G36" t="str">
-        <v>Ivanna I Gutierrez</v>
+        <v>Liliana Tumoine</v>
       </c>
       <c r="H36" t="str">
-        <v>Alejandra Villalobos</v>
+        <v>Olivia Zúñiga</v>
       </c>
       <c r="I36" t="str">
-        <v>Gaby Villarreal</v>
+        <v>Susy Rivera</v>
       </c>
     </row>
     <row r="37">
@@ -1462,28 +1462,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B37" t="str">
-        <v>19:30</v>
+        <v>17:00</v>
       </c>
       <c r="C37" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D37" t="str">
-        <v>TERCERA VARONIL</v>
+        <v>SUMA 5 VARONIL</v>
       </c>
       <c r="E37" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F37" t="str">
-        <v>Alberto Hermosillo</v>
+        <v>Josué Sánchez</v>
       </c>
       <c r="G37" t="str">
-        <v>Raul Urteaga</v>
+        <v>Patricio Murguia</v>
       </c>
       <c r="H37" t="str">
-        <v>Sonrics Moreno</v>
+        <v>Hugo Facio</v>
       </c>
       <c r="I37" t="str">
-        <v>Volker Muller</v>
+        <v>Eduardo Marin</v>
       </c>
     </row>
     <row r="38">
@@ -1491,7 +1491,7 @@
         <v>2025-10-26</v>
       </c>
       <c r="B38" t="str">
-        <v>19:30</v>
+        <v>17:00</v>
       </c>
       <c r="C38" t="str">
         <v>Múltiples canchas</v>
@@ -1503,16 +1503,16 @@
         <v>Jornada 2</v>
       </c>
       <c r="F38" t="str">
-        <v>Luis Mendoza</v>
+        <v>Rafael Reyes</v>
       </c>
       <c r="G38" t="str">
-        <v>Erick Martos</v>
+        <v>Andoni Esquivel</v>
       </c>
       <c r="H38" t="str">
-        <v>Sofia Salas</v>
+        <v>El Javi Fuentes</v>
       </c>
       <c r="I38" t="str">
-        <v>Luis Javier Gilio</v>
+        <v>Hector Becerra</v>
       </c>
     </row>
     <row r="39">
@@ -1520,28 +1520,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B39" t="str">
-        <v>20:45</v>
+        <v>18:15</v>
       </c>
       <c r="C39" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D39" t="str">
-        <v>SUMA 1 VARONIL</v>
+        <v>SUMA 3 FEMENIL</v>
       </c>
       <c r="E39" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F39" t="str">
-        <v>Carlos Niño de rivera</v>
+        <v>Isabel Rodriguez</v>
       </c>
       <c r="G39" t="str">
-        <v>Fernando Gonzalez</v>
+        <v>Cristina Fematt</v>
       </c>
       <c r="H39" t="str">
-        <v>Roberto Areco</v>
+        <v>Ximena Robles</v>
       </c>
       <c r="I39" t="str">
-        <v>Santiago Castiglioni</v>
+        <v>Romina Batarse</v>
       </c>
     </row>
     <row r="40">
@@ -1549,28 +1549,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B40" t="str">
-        <v>20:45</v>
+        <v>18:15</v>
       </c>
       <c r="C40" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D40" t="str">
-        <v>QUINTA VARONIL</v>
+        <v>SUMA 1 VARONIL</v>
       </c>
       <c r="E40" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F40" t="str">
-        <v>Omar Carrera</v>
+        <v>Marco Estefania</v>
       </c>
       <c r="G40" t="str">
-        <v>Francisco Recendiz</v>
+        <v>Andres Ollivier</v>
       </c>
       <c r="H40" t="str">
-        <v>ALFREDO PADILLA</v>
+        <v>Juan Francisco González</v>
       </c>
       <c r="I40" t="str">
-        <v>Luis Daniel Salazar</v>
+        <v>Mauricio Batres</v>
       </c>
     </row>
     <row r="41">
@@ -1578,28 +1578,28 @@
         <v>2025-10-26</v>
       </c>
       <c r="B41" t="str">
-        <v>20:45</v>
+        <v>18:15</v>
       </c>
       <c r="C41" t="str">
         <v>Múltiples canchas</v>
       </c>
       <c r="D41" t="str">
-        <v>QUINTA VARONIL</v>
+        <v>SUMA 3 FEMENIL</v>
       </c>
       <c r="E41" t="str">
         <v>Jornada 2</v>
       </c>
       <c r="F41" t="str">
-        <v>Jose Manuel Escapita</v>
+        <v>Daniela Peters</v>
       </c>
       <c r="G41" t="str">
-        <v>Marcelo García</v>
+        <v>Sandra Martinez</v>
       </c>
       <c r="H41" t="str">
-        <v>Sergio Dovalina</v>
+        <v>amina cassani</v>
       </c>
       <c r="I41" t="str">
-        <v>Wilbert Vladimi Alvarado</v>
+        <v>Andrea Quintero</v>
       </c>
     </row>
     <row r="42">
@@ -1607,33 +1607,613 @@
         <v>2025-10-26</v>
       </c>
       <c r="B42" t="str">
+        <v>18:15</v>
+      </c>
+      <c r="C42" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D42" t="str">
+        <v>SUMA 5 VARONIL</v>
+      </c>
+      <c r="E42" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F42" t="str">
+        <v>adrián fernandez</v>
+      </c>
+      <c r="G42" t="str">
+        <v>Roberto Soto</v>
+      </c>
+      <c r="H42" t="str">
+        <v>Fernando Gilio</v>
+      </c>
+      <c r="I42" t="str">
+        <v>Diego Rosales</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B43" t="str">
+        <v>18:15</v>
+      </c>
+      <c r="C43" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D43" t="str">
+        <v>SUMA 5 VARONIL</v>
+      </c>
+      <c r="E43" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F43" t="str">
+        <v>Carlos Mena</v>
+      </c>
+      <c r="G43" t="str">
+        <v>Elias Martinez</v>
+      </c>
+      <c r="H43" t="str">
+        <v>Mauricio Guizar</v>
+      </c>
+      <c r="I43" t="str">
+        <v>Humberto Ruiz</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B44" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D44" t="str">
+        <v>SUMA 3 FEMENIL</v>
+      </c>
+      <c r="E44" t="str">
+        <v>Jornada 1</v>
+      </c>
+      <c r="F44" t="str">
+        <v>Anilu Alvarado</v>
+      </c>
+      <c r="G44" t="str">
+        <v>Andrea Olivares</v>
+      </c>
+      <c r="H44" t="str">
+        <v>Susana Garza</v>
+      </c>
+      <c r="I44" t="str">
+        <v>Ana lucia Martinez</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B45" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D45" t="str">
+        <v>QUINTA VARONIL</v>
+      </c>
+      <c r="E45" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F45" t="str">
+        <v>Diego Fernandez</v>
+      </c>
+      <c r="G45" t="str">
+        <v>Ale Ramos</v>
+      </c>
+      <c r="H45" t="str">
+        <v>Raul Aguilar</v>
+      </c>
+      <c r="I45" t="str">
+        <v>Ernesto Sandoval</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B46" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D46" t="str">
+        <v>SUMA 3 FEMENIL</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F46" t="str">
+        <v>Isabella Cruz</v>
+      </c>
+      <c r="G46" t="str">
+        <v>Ivanna I Gutierrez</v>
+      </c>
+      <c r="H46" t="str">
+        <v>Alejandra Villalobos</v>
+      </c>
+      <c r="I46" t="str">
+        <v>Gaby Villarreal</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B47" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D47" t="str">
+        <v>TERCERA VARONIL</v>
+      </c>
+      <c r="E47" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F47" t="str">
+        <v>Alberto Hermosillo</v>
+      </c>
+      <c r="G47" t="str">
+        <v>Raul Urteaga</v>
+      </c>
+      <c r="H47" t="str">
+        <v>Sonrics Moreno</v>
+      </c>
+      <c r="I47" t="str">
+        <v>Volker Muller</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B48" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D48" t="str">
+        <v>SUMA 5 VARONIL</v>
+      </c>
+      <c r="E48" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F48" t="str">
+        <v>Luis Mendoza</v>
+      </c>
+      <c r="G48" t="str">
+        <v>Erick Martos</v>
+      </c>
+      <c r="H48" t="str">
+        <v>Sofia Salas</v>
+      </c>
+      <c r="I48" t="str">
+        <v>Luis Javier Gilio</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B49" t="str">
         <v>20:45</v>
       </c>
-      <c r="C42" t="str">
-        <v>Múltiples canchas</v>
-      </c>
-      <c r="D42" t="str">
+      <c r="C49" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D49" t="str">
         <v>QUINTA VARONIL</v>
       </c>
-      <c r="E42" t="str">
-        <v>Jornada 2</v>
-      </c>
-      <c r="F42" t="str">
+      <c r="E49" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F49" t="str">
+        <v>Luis Prieto</v>
+      </c>
+      <c r="G49" t="str">
+        <v>José Santiago Prieto</v>
+      </c>
+      <c r="H49" t="str">
+        <v>Miguel Rangel</v>
+      </c>
+      <c r="I49" t="str">
+        <v>Hector Cobos</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B50" t="str">
+        <v>20:45</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D50" t="str">
+        <v>SUMA 1 VARONIL</v>
+      </c>
+      <c r="E50" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F50" t="str">
+        <v>Carlos Niño de rivera</v>
+      </c>
+      <c r="G50" t="str">
+        <v>Fernando Gonzalez</v>
+      </c>
+      <c r="H50" t="str">
+        <v>Roberto Areco</v>
+      </c>
+      <c r="I50" t="str">
+        <v>Santiago Castiglioni</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B51" t="str">
+        <v>20:45</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D51" t="str">
+        <v>QUINTA VARONIL</v>
+      </c>
+      <c r="E51" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F51" t="str">
+        <v>Omar Carrera</v>
+      </c>
+      <c r="G51" t="str">
+        <v>Francisco Recendiz</v>
+      </c>
+      <c r="H51" t="str">
+        <v>ALFREDO PADILLA</v>
+      </c>
+      <c r="I51" t="str">
+        <v>Luis Daniel Salazar</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B52" t="str">
+        <v>20:45</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D52" t="str">
+        <v>QUINTA VARONIL</v>
+      </c>
+      <c r="E52" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F52" t="str">
+        <v>Jose Manuel Escapita</v>
+      </c>
+      <c r="G52" t="str">
+        <v>Marcelo García</v>
+      </c>
+      <c r="H52" t="str">
+        <v>Sergio Dovalina</v>
+      </c>
+      <c r="I52" t="str">
+        <v>Wilbert Vladimi Alvarado</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B53" t="str">
+        <v>20:45</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D53" t="str">
+        <v>QUINTA VARONIL</v>
+      </c>
+      <c r="E53" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F53" t="str">
         <v>Javier Meza</v>
       </c>
-      <c r="G42" t="str">
+      <c r="G53" t="str">
         <v>Eder Rodríguez</v>
       </c>
-      <c r="H42" t="str">
+      <c r="H53" t="str">
         <v>Sebastian Fernandez</v>
       </c>
-      <c r="I42" t="str">
+      <c r="I53" t="str">
         <v>Antonio Gilio</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B54" t="str">
+        <v>09:30</v>
+      </c>
+      <c r="C54" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D54" t="str">
+        <v>CUARTA VARONIL</v>
+      </c>
+      <c r="E54" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F54" t="str">
+        <v>Mauricio Tueme</v>
+      </c>
+      <c r="G54" t="str">
+        <v>arath tueme</v>
+      </c>
+      <c r="H54" t="str">
+        <v>Paco Amezcua</v>
+      </c>
+      <c r="I54" t="str">
+        <v>David Rangel</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B55" t="str">
+        <v>10:45</v>
+      </c>
+      <c r="C55" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D55" t="str">
+        <v>SENIORS 50+</v>
+      </c>
+      <c r="E55" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F55" t="str">
+        <v>Florencio Gil</v>
+      </c>
+      <c r="G55" t="str">
+        <v>Jorge Perez</v>
+      </c>
+      <c r="H55" t="str">
+        <v>Rick Campbell</v>
+      </c>
+      <c r="I55" t="str">
+        <v>Rayo Rodriguez</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B56" t="str">
+        <v>12:00</v>
+      </c>
+      <c r="C56" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D56" t="str">
+        <v>SUMA 9 FEMENIL</v>
+      </c>
+      <c r="E56" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F56" t="str">
+        <v>Laura Georgina Martínez</v>
+      </c>
+      <c r="G56" t="str">
+        <v>Damara Morales</v>
+      </c>
+      <c r="H56" t="str">
+        <v>Ana Isabel</v>
+      </c>
+      <c r="I56" t="str">
+        <v>Graciela Alba</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B57" t="str">
+        <v>13:15</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D57" t="str">
+        <v>CUARTA VARONIL</v>
+      </c>
+      <c r="E57" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F57" t="str">
+        <v>Pancho Ruiz</v>
+      </c>
+      <c r="G57" t="str">
+        <v>Francisco Ruiz</v>
+      </c>
+      <c r="H57" t="str">
+        <v>Fernando Gilio</v>
+      </c>
+      <c r="I57" t="str">
+        <v>Fernando Gilio</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B58" t="str">
+        <v>15:45</v>
+      </c>
+      <c r="C58" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D58" t="str">
+        <v>TERCERA VARONIL</v>
+      </c>
+      <c r="E58" t="str">
+        <v>Jornada 3</v>
+      </c>
+      <c r="F58" t="str">
+        <v>Daniel De Jesus Ortiz</v>
+      </c>
+      <c r="G58" t="str">
+        <v>Ricardo Garza</v>
+      </c>
+      <c r="H58" t="str">
+        <v>Manuel Ramirez</v>
+      </c>
+      <c r="I58" t="str">
+        <v>Chava Ruiz</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B59" t="str">
+        <v>17:00</v>
+      </c>
+      <c r="C59" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D59" t="str">
+        <v>SUMA 3 VARONIL</v>
+      </c>
+      <c r="E59" t="str">
+        <v>Jornada 1</v>
+      </c>
+      <c r="F59" t="str">
+        <v>Carlos “Charky” Alonzo</v>
+      </c>
+      <c r="G59" t="str">
+        <v>Carlo Rivas</v>
+      </c>
+      <c r="H59" t="str">
+        <v>Ricky Jr. Martínez</v>
+      </c>
+      <c r="I59" t="str">
+        <v>Jesus Martinez</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B60" t="str">
+        <v>18:15</v>
+      </c>
+      <c r="C60" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D60" t="str">
+        <v>CUARTA VARONIL</v>
+      </c>
+      <c r="E60" t="str">
+        <v>Jornada 3</v>
+      </c>
+      <c r="F60" t="str">
+        <v>Iván Rangel</v>
+      </c>
+      <c r="G60" t="str">
+        <v>Fernando Pámanes</v>
+      </c>
+      <c r="H60" t="str">
+        <v>Roberto Ibarra</v>
+      </c>
+      <c r="I60" t="str">
+        <v>Federico Garza</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B61" t="str">
+        <v>19:30</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D61" t="str">
+        <v>QUINTA FEMENIL</v>
+      </c>
+      <c r="E61" t="str">
+        <v>Jornada 1</v>
+      </c>
+      <c r="F61" t="str">
+        <v>Ana Isabel</v>
+      </c>
+      <c r="G61" t="str">
+        <v>Mayte Nuñez</v>
+      </c>
+      <c r="H61" t="str">
+        <v>Christa Del hoyo</v>
+      </c>
+      <c r="I61" t="str">
+        <v>Mariana Acosta</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>2025-10-26</v>
+      </c>
+      <c r="B62" t="str">
+        <v>20:45</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Múltiples canchas</v>
+      </c>
+      <c r="D62" t="str">
+        <v>SUMA 3 VARONIL</v>
+      </c>
+      <c r="E62" t="str">
+        <v>Jornada 2</v>
+      </c>
+      <c r="F62" t="str">
+        <v>Ruben Aguiñaga</v>
+      </c>
+      <c r="G62" t="str">
+        <v>Alejandro Aguiñaga</v>
+      </c>
+      <c r="H62" t="str">
+        <v>Jorge Chibli</v>
+      </c>
+      <c r="I62" t="str">
+        <v>Marco Estefania</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I62"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>